<commit_message>
Changed starting Cell in excel write range
</commit_message>
<xml_diff>
--- a/book1.xlsx
+++ b/book1.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/469f30f3a5a2c5d1/Dokumenty/UiPath/WeatherAPI/WeatherAPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A7268C-8C00-46F3-B1E3-ADC6CC29DE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{46A7268C-8C00-46F3-B1E3-ADC6CC29DE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2445DB53-3C88-4AA9-9FD5-E4D64D7EF628}"/>
   <bookViews>
     <workbookView xWindow="-24930" yWindow="765" windowWidth="20460" windowHeight="11835" xr2:uid="{D9B94B64-EF2E-4F51-9658-06048CD51DE3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="5" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,11 +26,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Location</t>
   </si>
   <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Sky</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
     <t>london</t>
   </si>
   <si>
@@ -39,22 +52,64 @@
     <t>paris</t>
   </si>
   <si>
+    <t>madrit</t>
+  </si>
+  <si>
     <t>budapest</t>
   </si>
   <si>
-    <t>madrit</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Sky</t>
-  </si>
-  <si>
-    <t>Humidity</t>
-  </si>
-  <si>
-    <t>Wind</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Klart</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>7 m/s Sydvest</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Skyet</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>3 m/s Syd</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>3 m/s Vest</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>1 m/s Nordvest</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Mest skyet</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>2 m/s Øst</t>
   </si>
 </sst>
 </file>
@@ -91,8 +146,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -406,58 +462,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0767556C-15CC-460A-9AA6-E6E372383115}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>